<commit_message>
add more jer days
</commit_message>
<xml_diff>
--- a/data/bible-in-year-fr-mike.xlsx
+++ b/data/bible-in-year-fr-mike.xlsx
@@ -20151,10 +20151,10 @@
         </is>
       </c>
       <c r="E237" t="n">
-        <v>0</v>
+        <v>87</v>
       </c>
       <c r="F237" t="n">
-        <v>0</v>
+        <v>553</v>
       </c>
       <c r="G237" t="inlineStr">
         <is>
@@ -20162,10 +20162,10 @@
         </is>
       </c>
       <c r="H237" t="n">
-        <v>0</v>
+        <v>554</v>
       </c>
       <c r="I237" t="n">
-        <v>0</v>
+        <v>1068</v>
       </c>
       <c r="J237" t="inlineStr">
         <is>
@@ -20173,19 +20173,19 @@
         </is>
       </c>
       <c r="K237" t="n">
-        <v>0</v>
+        <v>1070</v>
       </c>
       <c r="L237" t="n">
-        <v>0</v>
+        <v>1101</v>
       </c>
       <c r="M237" t="n">
-        <v>0</v>
+        <v>1103</v>
       </c>
       <c r="N237" t="n">
-        <v>0</v>
+        <v>1187</v>
       </c>
       <c r="O237" t="n">
-        <v>0</v>
+        <v>1188</v>
       </c>
       <c r="P237" t="n">
         <v>1768</v>
@@ -20236,10 +20236,10 @@
         </is>
       </c>
       <c r="E238" t="n">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="F238" t="n">
-        <v>0</v>
+        <v>424</v>
       </c>
       <c r="G238" t="inlineStr">
         <is>
@@ -20247,10 +20247,10 @@
         </is>
       </c>
       <c r="H238" t="n">
-        <v>0</v>
+        <v>426</v>
       </c>
       <c r="I238" t="n">
-        <v>0</v>
+        <v>954</v>
       </c>
       <c r="J238" t="inlineStr">
         <is>
@@ -20258,19 +20258,19 @@
         </is>
       </c>
       <c r="K238" t="n">
-        <v>0</v>
+        <v>956</v>
       </c>
       <c r="L238" t="n">
-        <v>0</v>
+        <v>986</v>
       </c>
       <c r="M238" t="n">
-        <v>0</v>
+        <v>988</v>
       </c>
       <c r="N238" t="n">
-        <v>0</v>
+        <v>1027</v>
       </c>
       <c r="O238" t="n">
-        <v>0</v>
+        <v>1028</v>
       </c>
       <c r="P238" t="n">
         <v>1633</v>
@@ -20321,10 +20321,10 @@
         </is>
       </c>
       <c r="E239" t="n">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="F239" t="n">
-        <v>0</v>
+        <v>418</v>
       </c>
       <c r="G239" t="inlineStr">
         <is>
@@ -20332,10 +20332,10 @@
         </is>
       </c>
       <c r="H239" t="n">
-        <v>0</v>
+        <v>420</v>
       </c>
       <c r="I239" t="n">
-        <v>0</v>
+        <v>1035</v>
       </c>
       <c r="J239" t="inlineStr">
         <is>
@@ -20343,19 +20343,19 @@
         </is>
       </c>
       <c r="K239" t="n">
-        <v>0</v>
+        <v>1037</v>
       </c>
       <c r="L239" t="n">
-        <v>0</v>
+        <v>1067</v>
       </c>
       <c r="M239" t="n">
-        <v>0</v>
+        <v>1069</v>
       </c>
       <c r="N239" t="n">
-        <v>0</v>
+        <v>1109</v>
       </c>
       <c r="O239" t="n">
-        <v>0</v>
+        <v>1110</v>
       </c>
       <c r="P239" t="n">
         <v>1763</v>
@@ -20406,10 +20406,10 @@
         </is>
       </c>
       <c r="E240" t="n">
-        <v>0</v>
+        <v>77</v>
       </c>
       <c r="F240" t="n">
-        <v>0</v>
+        <v>351</v>
       </c>
       <c r="G240" t="inlineStr">
         <is>
@@ -20417,10 +20417,10 @@
         </is>
       </c>
       <c r="H240" t="n">
-        <v>0</v>
+        <v>353</v>
       </c>
       <c r="I240" t="n">
-        <v>0</v>
+        <v>1118</v>
       </c>
       <c r="J240" t="inlineStr">
         <is>
@@ -20428,19 +20428,19 @@
         </is>
       </c>
       <c r="K240" t="n">
-        <v>0</v>
+        <v>1121</v>
       </c>
       <c r="L240" t="n">
-        <v>0</v>
+        <v>1154</v>
       </c>
       <c r="M240" t="n">
-        <v>0</v>
+        <v>1157</v>
       </c>
       <c r="N240" t="n">
-        <v>0</v>
+        <v>1188</v>
       </c>
       <c r="O240" t="n">
-        <v>0</v>
+        <v>1189</v>
       </c>
       <c r="P240" t="n">
         <v>1734</v>
@@ -20491,10 +20491,10 @@
         </is>
       </c>
       <c r="E241" t="n">
-        <v>0</v>
+        <v>92</v>
       </c>
       <c r="F241" t="n">
-        <v>0</v>
+        <v>471</v>
       </c>
       <c r="G241" t="inlineStr">
         <is>
@@ -20502,10 +20502,10 @@
         </is>
       </c>
       <c r="H241" t="n">
-        <v>0</v>
+        <v>473</v>
       </c>
       <c r="I241" t="n">
-        <v>0</v>
+        <v>1167</v>
       </c>
       <c r="J241" t="inlineStr">
         <is>
@@ -20513,19 +20513,19 @@
         </is>
       </c>
       <c r="K241" t="n">
-        <v>0</v>
+        <v>1169</v>
       </c>
       <c r="L241" t="n">
-        <v>0</v>
+        <v>1201</v>
       </c>
       <c r="M241" t="n">
-        <v>0</v>
+        <v>1203</v>
       </c>
       <c r="N241" t="n">
-        <v>0</v>
+        <v>1264</v>
       </c>
       <c r="O241" t="n">
-        <v>0</v>
+        <v>1265</v>
       </c>
       <c r="P241" t="n">
         <v>1606</v>
@@ -20576,10 +20576,10 @@
         </is>
       </c>
       <c r="E242" t="n">
-        <v>0</v>
+        <v>61</v>
       </c>
       <c r="F242" t="n">
-        <v>0</v>
+        <v>474</v>
       </c>
       <c r="G242" t="inlineStr">
         <is>
@@ -20587,10 +20587,10 @@
         </is>
       </c>
       <c r="H242" t="n">
-        <v>0</v>
+        <v>476</v>
       </c>
       <c r="I242" t="n">
-        <v>0</v>
+        <v>1031</v>
       </c>
       <c r="J242" t="inlineStr">
         <is>
@@ -20598,19 +20598,19 @@
         </is>
       </c>
       <c r="K242" t="n">
-        <v>0</v>
+        <v>1033</v>
       </c>
       <c r="L242" t="n">
-        <v>0</v>
+        <v>1063</v>
       </c>
       <c r="M242" t="n">
-        <v>0</v>
+        <v>1065</v>
       </c>
       <c r="N242" t="n">
-        <v>0</v>
+        <v>1099</v>
       </c>
       <c r="O242" t="n">
-        <v>0</v>
+        <v>1100</v>
       </c>
       <c r="P242" t="n">
         <v>1730</v>

</xml_diff>